<commit_message>
added plots readme update, text_prace added
</commit_message>
<xml_diff>
--- a/plots_tabs/metrics.xlsx
+++ b/plots_tabs/metrics.xlsx
@@ -1,21 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jezva\Desktop\R\Projekty\cara_stock_pred\plots_tabs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA719F7-D951-42DB-8996-81004908B94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="51480" yWindow="6495" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MASE</t>
+  </si>
+  <si>
+    <t>arima</t>
+  </si>
+  <si>
+    <t>arimax</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>varx</t>
+  </si>
+  <si>
+    <t>naive</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,17 +100,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +156,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,130 +401,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>MSE</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>MAE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>MASE</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>arima</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0.00141233538797599</v>
+        <v>1.4479556129399899E-3</v>
       </c>
       <c r="C2">
-        <v>0.03758105091633268</v>
+        <v>3.8052011943391237E-2</v>
       </c>
       <c r="D2">
-        <v>0.0263191008672758</v>
+        <v>2.6704623427587181E-2</v>
       </c>
       <c r="E2">
-        <v>0.6819609376917984</v>
+        <v>0.68234672134990504</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>arimax</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0.001428196207733864</v>
+        <v>1.464577242493714E-3</v>
       </c>
       <c r="C3">
-        <v>0.03779148326983031</v>
+        <v>3.8269795433131262E-2</v>
       </c>
       <c r="D3">
-        <v>0.02645638645670933</v>
+        <v>2.6838237258797921E-2</v>
       </c>
       <c r="E3">
-        <v>0.6855181796269917</v>
+        <v>0.68576077284929682</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>var</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.001425795390969145</v>
+        <v>1.463096896369838E-3</v>
       </c>
       <c r="C4">
-        <v>0.03775970591740811</v>
+        <v>3.8250449623106898E-2</v>
       </c>
       <c r="D4">
-        <v>0.02670953958018954</v>
+        <v>2.7100211991287839E-2</v>
       </c>
       <c r="E4">
-        <v>0.692077694799595</v>
+        <v>0.69245465491341729</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>varx</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>0.00144000948240071</v>
+        <v>1.477500091158331E-3</v>
       </c>
       <c r="C5">
-        <v>0.03794745686341458</v>
+        <v>3.8438263373341039E-2</v>
       </c>
       <c r="D5">
-        <v>0.02684483283168022</v>
+        <v>2.724523860907797E-2</v>
       </c>
       <c r="E5">
-        <v>0.6955833127580215</v>
+        <v>0.69616032174020848</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>naive</t>
-        </is>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>0.002841551316829281</v>
+        <v>2.9150351947141188E-3</v>
       </c>
       <c r="C6">
-        <v>0.05330620336160963</v>
+        <v>5.3991065878662918E-2</v>
       </c>
       <c r="D6">
-        <v>0.03859326746243977</v>
+        <v>3.9136442796642593E-2</v>
       </c>
       <c r="E6">
         <v>1</v>

</xml_diff>